<commit_message>
Add student's missed sessions to database
</commit_message>
<xml_diff>
--- a/static/excel/samples/student_bio_data.xlsx
+++ b/static/excel/samples/student_bio_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0BCF88-D24C-4006-B031-DAE93C69499F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39146C02-D176-48AF-8B95-482C1F5B62B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Matric NO</t>
   </si>
@@ -79,10 +79,16 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>State</t>
+    <t>U2015/3025000</t>
   </si>
   <si>
-    <t>U2015/3025000</t>
+    <t>Rivers</t>
+  </si>
+  <si>
+    <t>Missed Sessions</t>
+  </si>
+  <si>
+    <t>2015/2016, 2016/2017, 2017/2018</t>
   </si>
 </sst>
 </file>
@@ -126,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -158,6 +164,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -165,7 +191,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -175,12 +201,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number Style" xfId="1" xr:uid="{3F35957B-008B-4DD5-888E-1BF85505A66E}"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -293,6 +336,13 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -318,13 +368,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
       </border>
     </dxf>
     <dxf>
@@ -364,9 +407,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Semester Style" pivot="0" count="3" xr9:uid="{76CBB96B-0C45-4CF6-A9BA-2FA186E32BFA}">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="totalRow" dxfId="11"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -381,19 +424,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7BAF8AF9-FE7E-4C26-9CE5-39B51F7A0A6F}" name="Table3" displayName="Table3" ref="A1:I251" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="10">
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{03666201-703C-4511-955E-41CFD2A5964C}" name="S/N" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7BAF8AF9-FE7E-4C26-9CE5-39B51F7A0A6F}" name="Table3" displayName="Table3" ref="A1:J251" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{03666201-703C-4511-955E-41CFD2A5964C}" name="S/N" dataDxfId="9">
       <calculatedColumnFormula>ROW()-ROW(S_N)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A4F45E95-3E87-4B8D-948D-CBC14E8BE626}" name="Matric NO" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{5654AEB4-E02D-46F2-9097-268CC0AA5555}" name="First Name" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4B079751-EAF1-4002-9342-AB8C668AED98}" name="Last Name" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{610752AC-CE04-44A9-8522-7A50EA38594A}" name="Other Names" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{8DA555E0-9C62-4F9F-A965-3CAC2E10D1B3}" name="Department" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{0543A9BF-C2F0-4261-A622-B5F2375F163E}" name="Sex" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{56AF198A-6CBE-4431-A8D6-7600C3EF332C}" name="State of Origin" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{659CEECD-EEAE-4A20-B4C0-9A931DA6805B}" name="Marital Status" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{A4F45E95-3E87-4B8D-948D-CBC14E8BE626}" name="Matric NO" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{5654AEB4-E02D-46F2-9097-268CC0AA5555}" name="First Name" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4B079751-EAF1-4002-9342-AB8C668AED98}" name="Last Name" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{610752AC-CE04-44A9-8522-7A50EA38594A}" name="Other Names" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{8DA555E0-9C62-4F9F-A965-3CAC2E10D1B3}" name="Department" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{0543A9BF-C2F0-4261-A622-B5F2375F163E}" name="Sex" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{56AF198A-6CBE-4431-A8D6-7600C3EF332C}" name="State of Origin" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{659CEECD-EEAE-4A20-B4C0-9A931DA6805B}" name="Marital Status" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{BF72F716-1468-45D7-867F-EC38F8392790}" name="Missed Sessions" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Semester Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -662,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I253"/>
+  <dimension ref="A1:J253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -679,9 +723,10 @@
     <col min="7" max="7" width="5.40625" customWidth="1"/>
     <col min="8" max="8" width="14.6328125" customWidth="1"/>
     <col min="9" max="9" width="14.36328125" customWidth="1"/>
+    <col min="10" max="10" width="32.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -709,14 +754,17 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" ref="A2:A65" si="0">ROW()-ROW(S_N)</f>
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -732,15 +780,18 @@
         <v>9</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
@@ -751,10 +802,11 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
@@ -765,10 +817,11 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
@@ -779,10 +832,11 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="3"/>
@@ -793,10 +847,11 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
@@ -807,10 +862,11 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
@@ -821,10 +877,11 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
@@ -835,10 +892,11 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
@@ -849,10 +907,11 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="3"/>
@@ -863,10 +922,11 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="3"/>
@@ -877,10 +937,11 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="3"/>
@@ -891,10 +952,11 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
@@ -905,10 +967,11 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
@@ -919,10 +982,11 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="3"/>
@@ -933,10 +997,11 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A17">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="3"/>
@@ -947,10 +1012,11 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A18">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="3"/>
@@ -961,10 +1027,11 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A19">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="3"/>
@@ -975,10 +1042,11 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A20">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="3"/>
@@ -989,10 +1057,11 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A21">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="3"/>
@@ -1003,10 +1072,11 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A22">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="3"/>
@@ -1017,10 +1087,11 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A23">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="3"/>
@@ -1031,10 +1102,11 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A24">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="3"/>
@@ -1045,10 +1117,11 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A25">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="3"/>
@@ -1059,10 +1132,11 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A26">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="3"/>
@@ -1073,10 +1147,11 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A27">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="3"/>
@@ -1087,10 +1162,11 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A28">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="3"/>
@@ -1101,10 +1177,11 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A29">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="3"/>
@@ -1115,10 +1192,11 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A30">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="3"/>
@@ -1129,10 +1207,11 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A31">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="3"/>
@@ -1143,10 +1222,11 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A32">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="3"/>
@@ -1157,10 +1237,11 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A33">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="3"/>
@@ -1171,10 +1252,11 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A34">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="3"/>
@@ -1185,10 +1267,11 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A35">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="3"/>
@@ -1199,10 +1282,11 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A36">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="3"/>
@@ -1213,10 +1297,11 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A37">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="3"/>
@@ -1227,10 +1312,11 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A38">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="3"/>
@@ -1241,10 +1327,11 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A39">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" s="3"/>
@@ -1255,10 +1342,11 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A40">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="3"/>
@@ -1269,10 +1357,11 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A41">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" s="3"/>
@@ -1283,10 +1372,11 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A42">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" s="3"/>
@@ -1297,10 +1387,11 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A43">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" s="3"/>
@@ -1311,10 +1402,11 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A44">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" s="3"/>
@@ -1325,10 +1417,11 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A45">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" s="3"/>
@@ -1339,10 +1432,11 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A46">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" s="3"/>
@@ -1353,10 +1447,11 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A47">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" s="3"/>
@@ -1367,10 +1462,11 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A48">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" s="3"/>
@@ -1381,10 +1477,11 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A49">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" s="3"/>
@@ -1395,10 +1492,11 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A50">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" s="3"/>
@@ -1409,10 +1507,11 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A51">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51" s="3"/>
@@ -1423,10 +1522,11 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A52">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" s="3"/>
@@ -1437,10 +1537,11 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A53">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" s="3"/>
@@ -1451,10 +1552,11 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A54">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" s="3"/>
@@ -1465,10 +1567,11 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A55">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" s="3"/>
@@ -1479,10 +1582,11 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A56">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" s="3"/>
@@ -1493,10 +1597,11 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A57">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" s="3"/>
@@ -1507,10 +1612,11 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A58">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B58" s="3"/>
@@ -1521,10 +1627,11 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A59">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B59" s="3"/>
@@ -1535,10 +1642,11 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A60">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B60" s="3"/>
@@ -1549,10 +1657,11 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A61">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B61" s="3"/>
@@ -1563,10 +1672,11 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A62">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B62" s="3"/>
@@ -1577,10 +1687,11 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A63">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B63" s="3"/>
@@ -1591,10 +1702,11 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A64">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B64" s="3"/>
@@ -1605,10 +1717,11 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A65">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B65" s="3"/>
@@ -1619,10 +1732,11 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A66">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" ref="A66:A129" si="1">ROW()-ROW(S_N)</f>
         <v>65</v>
       </c>
       <c r="B66" s="3"/>
@@ -1633,10 +1747,11 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A67">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="B67" s="3"/>
@@ -1647,10 +1762,11 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A68">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="B68" s="3"/>
@@ -1661,10 +1777,11 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A69">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="B69" s="3"/>
@@ -1675,10 +1792,11 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A70">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="B70" s="3"/>
@@ -1689,10 +1807,11 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A71">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B71" s="3"/>
@@ -1703,10 +1822,11 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A72">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="B72" s="3"/>
@@ -1717,10 +1837,11 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A73">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="B73" s="3"/>
@@ -1731,10 +1852,11 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A74">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="B74" s="3"/>
@@ -1745,10 +1867,11 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A75">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="B75" s="3"/>
@@ -1759,10 +1882,11 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A76">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="B76" s="3"/>
@@ -1773,10 +1897,11 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A77">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="B77" s="3"/>
@@ -1787,10 +1912,11 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A78">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="B78" s="3"/>
@@ -1801,10 +1927,11 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J78" s="5"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A79">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="B79" s="3"/>
@@ -1815,10 +1942,11 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A80">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>79</v>
       </c>
       <c r="B80" s="3"/>
@@ -1829,10 +1957,11 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A81">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="B81" s="3"/>
@@ -1843,10 +1972,11 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J81" s="5"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A82">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="B82" s="3"/>
@@ -1857,10 +1987,11 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J82" s="5"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A83">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="B83" s="3"/>
@@ -1871,10 +2002,11 @@
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J83" s="5"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A84">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="B84" s="3"/>
@@ -1885,10 +2017,11 @@
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A85">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="B85" s="3"/>
@@ -1899,10 +2032,11 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A86">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="B86" s="3"/>
@@ -1913,10 +2047,11 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J86" s="5"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A87">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="B87" s="3"/>
@@ -1927,10 +2062,11 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J87" s="5"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A88">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="B88" s="3"/>
@@ -1941,10 +2077,11 @@
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J88" s="5"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A89">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="B89" s="3"/>
@@ -1955,10 +2092,11 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J89" s="5"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A90">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="B90" s="3"/>
@@ -1969,10 +2107,11 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J90" s="5"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A91">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="B91" s="3"/>
@@ -1983,10 +2122,11 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J91" s="5"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A92">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>91</v>
       </c>
       <c r="B92" s="3"/>
@@ -1997,10 +2137,11 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J92" s="5"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A93">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="B93" s="3"/>
@@ -2011,10 +2152,11 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J93" s="5"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A94">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
       <c r="B94" s="3"/>
@@ -2025,10 +2167,11 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J94" s="5"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A95">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
       <c r="B95" s="3"/>
@@ -2039,10 +2182,11 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J95" s="5"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A96">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="B96" s="3"/>
@@ -2053,10 +2197,11 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J96" s="5"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A97">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="B97" s="3"/>
@@ -2067,10 +2212,11 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J97" s="5"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A98">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
       <c r="B98" s="3"/>
@@ -2081,10 +2227,11 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J98" s="5"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A99">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="B99" s="3"/>
@@ -2095,10 +2242,11 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J99" s="5"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A100">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
       <c r="B100" s="3"/>
@@ -2109,10 +2257,11 @@
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J100" s="5"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A101">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="B101" s="3"/>
@@ -2123,10 +2272,11 @@
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J101" s="5"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A102">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>101</v>
       </c>
       <c r="B102" s="3"/>
@@ -2137,10 +2287,11 @@
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J102" s="5"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A103">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="B103" s="3"/>
@@ -2151,10 +2302,11 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J103" s="5"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A104">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="B104" s="3"/>
@@ -2165,10 +2317,11 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J104" s="5"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A105">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
       <c r="B105" s="3"/>
@@ -2179,10 +2332,11 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J105" s="5"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A106">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="B106" s="3"/>
@@ -2193,10 +2347,11 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J106" s="5"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A107">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="B107" s="3"/>
@@ -2207,10 +2362,11 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J107" s="5"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A108">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="B108" s="3"/>
@@ -2221,10 +2377,11 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J108" s="5"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A109">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>108</v>
       </c>
       <c r="B109" s="3"/>
@@ -2235,10 +2392,11 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A110">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>109</v>
       </c>
       <c r="B110" s="3"/>
@@ -2249,10 +2407,11 @@
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A111">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="B111" s="3"/>
@@ -2263,10 +2422,11 @@
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J111" s="5"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A112">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="B112" s="3"/>
@@ -2277,10 +2437,11 @@
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J112" s="5"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A113">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="B113" s="3"/>
@@ -2291,10 +2452,11 @@
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J113" s="5"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A114">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>113</v>
       </c>
       <c r="B114" s="3"/>
@@ -2305,10 +2467,11 @@
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J114" s="5"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A115">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>114</v>
       </c>
       <c r="B115" s="3"/>
@@ -2319,10 +2482,11 @@
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J115" s="5"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A116">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="B116" s="3"/>
@@ -2333,10 +2497,11 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J116" s="5"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A117">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="B117" s="3"/>
@@ -2347,10 +2512,11 @@
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J117" s="5"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A118">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="B118" s="3"/>
@@ -2361,10 +2527,11 @@
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J118" s="5"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A119">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="B119" s="3"/>
@@ -2375,10 +2542,11 @@
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J119" s="5"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A120">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>119</v>
       </c>
       <c r="B120" s="3"/>
@@ -2389,10 +2557,11 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J120" s="5"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A121">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="B121" s="3"/>
@@ -2403,10 +2572,11 @@
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J121" s="5"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A122">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>121</v>
       </c>
       <c r="B122" s="3"/>
@@ -2417,10 +2587,11 @@
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J122" s="5"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A123">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>122</v>
       </c>
       <c r="B123" s="3"/>
@@ -2431,10 +2602,11 @@
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J123" s="5"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A124">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="B124" s="3"/>
@@ -2445,10 +2617,11 @@
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J124" s="5"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A125">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="B125" s="3"/>
@@ -2459,10 +2632,11 @@
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J125" s="5"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A126">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
       <c r="B126" s="3"/>
@@ -2473,10 +2647,11 @@
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J126" s="5"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A127">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>126</v>
       </c>
       <c r="B127" s="3"/>
@@ -2487,10 +2662,11 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J127" s="5"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A128">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="B128" s="3"/>
@@ -2501,10 +2677,11 @@
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J128" s="5"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A129">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="B129" s="3"/>
@@ -2515,10 +2692,11 @@
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J129" s="5"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A130">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" ref="A130:A193" si="2">ROW()-ROW(S_N)</f>
         <v>129</v>
       </c>
       <c r="B130" s="3"/>
@@ -2529,10 +2707,11 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J130" s="5"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A131">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="B131" s="3"/>
@@ -2543,10 +2722,11 @@
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J131" s="5"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A132">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>131</v>
       </c>
       <c r="B132" s="3"/>
@@ -2557,10 +2737,11 @@
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J132" s="5"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A133">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="B133" s="3"/>
@@ -2571,10 +2752,11 @@
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J133" s="5"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A134">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>133</v>
       </c>
       <c r="B134" s="3"/>
@@ -2585,10 +2767,11 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J134" s="5"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A135">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>134</v>
       </c>
       <c r="B135" s="3"/>
@@ -2599,10 +2782,11 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J135" s="5"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A136">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>135</v>
       </c>
       <c r="B136" s="3"/>
@@ -2613,10 +2797,11 @@
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J136" s="5"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A137">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>136</v>
       </c>
       <c r="B137" s="3"/>
@@ -2627,10 +2812,11 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J137" s="5"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A138">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>137</v>
       </c>
       <c r="B138" s="3"/>
@@ -2641,10 +2827,11 @@
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J138" s="5"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A139">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="B139" s="3"/>
@@ -2655,10 +2842,11 @@
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J139" s="5"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A140">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>139</v>
       </c>
       <c r="B140" s="3"/>
@@ -2669,10 +2857,11 @@
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J140" s="5"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A141">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
       <c r="B141" s="3"/>
@@ -2683,10 +2872,11 @@
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J141" s="5"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A142">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>141</v>
       </c>
       <c r="B142" s="3"/>
@@ -2697,10 +2887,11 @@
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J142" s="5"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A143">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="B143" s="3"/>
@@ -2711,10 +2902,11 @@
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J143" s="5"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A144">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>143</v>
       </c>
       <c r="B144" s="3"/>
@@ -2725,10 +2917,11 @@
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J144" s="5"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A145">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="B145" s="3"/>
@@ -2739,10 +2932,11 @@
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J145" s="5"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A146">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>145</v>
       </c>
       <c r="B146" s="3"/>
@@ -2753,10 +2947,11 @@
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J146" s="5"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A147">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>146</v>
       </c>
       <c r="B147" s="3"/>
@@ -2767,10 +2962,11 @@
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J147" s="5"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A148">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
       <c r="B148" s="3"/>
@@ -2781,10 +2977,11 @@
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J148" s="5"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A149">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="B149" s="3"/>
@@ -2795,10 +2992,11 @@
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J149" s="5"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A150">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>149</v>
       </c>
       <c r="B150" s="3"/>
@@ -2809,10 +3007,11 @@
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J150" s="5"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A151">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="B151" s="3"/>
@@ -2823,10 +3022,11 @@
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J151" s="5"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A152">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>151</v>
       </c>
       <c r="B152" s="3"/>
@@ -2837,10 +3037,11 @@
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J152" s="5"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A153">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>152</v>
       </c>
       <c r="B153" s="3"/>
@@ -2851,10 +3052,11 @@
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J153" s="5"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A154">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>153</v>
       </c>
       <c r="B154" s="3"/>
@@ -2865,10 +3067,11 @@
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J154" s="5"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A155">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>154</v>
       </c>
       <c r="B155" s="3"/>
@@ -2879,10 +3082,11 @@
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J155" s="5"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A156">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="B156" s="3"/>
@@ -2893,10 +3097,11 @@
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J156" s="5"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A157">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="B157" s="3"/>
@@ -2907,10 +3112,11 @@
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J157" s="5"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A158">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="B158" s="3"/>
@@ -2921,10 +3127,11 @@
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J158" s="5"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A159">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>158</v>
       </c>
       <c r="B159" s="3"/>
@@ -2935,10 +3142,11 @@
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J159" s="5"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A160">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>159</v>
       </c>
       <c r="B160" s="3"/>
@@ -2949,10 +3157,11 @@
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J160" s="5"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A161">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="B161" s="3"/>
@@ -2963,10 +3172,11 @@
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J161" s="5"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A162">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>161</v>
       </c>
       <c r="B162" s="3"/>
@@ -2977,10 +3187,11 @@
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J162" s="5"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A163">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>162</v>
       </c>
       <c r="B163" s="3"/>
@@ -2991,10 +3202,11 @@
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J163" s="5"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A164">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>163</v>
       </c>
       <c r="B164" s="3"/>
@@ -3005,10 +3217,11 @@
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J164" s="5"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A165">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="B165" s="3"/>
@@ -3019,10 +3232,11 @@
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J165" s="5"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A166">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="B166" s="3"/>
@@ -3033,10 +3247,11 @@
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J166" s="5"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A167">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>166</v>
       </c>
       <c r="B167" s="3"/>
@@ -3047,10 +3262,11 @@
       <c r="G167" s="3"/>
       <c r="H167" s="3"/>
       <c r="I167" s="3"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J167" s="5"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A168">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>167</v>
       </c>
       <c r="B168" s="3"/>
@@ -3061,10 +3277,11 @@
       <c r="G168" s="3"/>
       <c r="H168" s="3"/>
       <c r="I168" s="3"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J168" s="5"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A169">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>168</v>
       </c>
       <c r="B169" s="3"/>
@@ -3075,10 +3292,11 @@
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
       <c r="I169" s="3"/>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J169" s="5"/>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A170">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="B170" s="3"/>
@@ -3089,10 +3307,11 @@
       <c r="G170" s="3"/>
       <c r="H170" s="3"/>
       <c r="I170" s="3"/>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J170" s="5"/>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A171">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="B171" s="3"/>
@@ -3103,10 +3322,11 @@
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
       <c r="I171" s="3"/>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J171" s="5"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A172">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>171</v>
       </c>
       <c r="B172" s="3"/>
@@ -3117,10 +3337,11 @@
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
       <c r="I172" s="3"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J172" s="5"/>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A173">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>172</v>
       </c>
       <c r="B173" s="3"/>
@@ -3131,10 +3352,11 @@
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
       <c r="I173" s="3"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J173" s="5"/>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A174">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>173</v>
       </c>
       <c r="B174" s="3"/>
@@ -3145,10 +3367,11 @@
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
       <c r="I174" s="3"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J174" s="5"/>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A175">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>174</v>
       </c>
       <c r="B175" s="3"/>
@@ -3159,10 +3382,11 @@
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
       <c r="I175" s="3"/>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J175" s="5"/>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A176">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>175</v>
       </c>
       <c r="B176" s="3"/>
@@ -3173,10 +3397,11 @@
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
       <c r="I176" s="3"/>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J176" s="5"/>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A177">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="B177" s="3"/>
@@ -3187,10 +3412,11 @@
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
       <c r="I177" s="3"/>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J177" s="5"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A178">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>177</v>
       </c>
       <c r="B178" s="3"/>
@@ -3201,10 +3427,11 @@
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J178" s="5"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A179">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>178</v>
       </c>
       <c r="B179" s="3"/>
@@ -3215,10 +3442,11 @@
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
       <c r="I179" s="3"/>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J179" s="5"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A180">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>179</v>
       </c>
       <c r="B180" s="3"/>
@@ -3229,10 +3457,11 @@
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
       <c r="I180" s="3"/>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J180" s="5"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A181">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="B181" s="3"/>
@@ -3243,10 +3472,11 @@
       <c r="G181" s="3"/>
       <c r="H181" s="3"/>
       <c r="I181" s="3"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J181" s="5"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A182">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="B182" s="3"/>
@@ -3257,10 +3487,11 @@
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
       <c r="I182" s="3"/>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J182" s="5"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A183">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>182</v>
       </c>
       <c r="B183" s="3"/>
@@ -3271,10 +3502,11 @@
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
       <c r="I183" s="3"/>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J183" s="5"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A184">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>183</v>
       </c>
       <c r="B184" s="3"/>
@@ -3285,10 +3517,11 @@
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
       <c r="I184" s="3"/>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J184" s="5"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A185">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>184</v>
       </c>
       <c r="B185" s="3"/>
@@ -3299,10 +3532,11 @@
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
       <c r="I185" s="3"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J185" s="5"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A186">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>185</v>
       </c>
       <c r="B186" s="3"/>
@@ -3313,10 +3547,11 @@
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
       <c r="I186" s="3"/>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J186" s="5"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A187">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>186</v>
       </c>
       <c r="B187" s="3"/>
@@ -3327,10 +3562,11 @@
       <c r="G187" s="3"/>
       <c r="H187" s="3"/>
       <c r="I187" s="3"/>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J187" s="5"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A188">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>187</v>
       </c>
       <c r="B188" s="3"/>
@@ -3341,10 +3577,11 @@
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
       <c r="I188" s="3"/>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J188" s="5"/>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A189">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>188</v>
       </c>
       <c r="B189" s="3"/>
@@ -3355,10 +3592,11 @@
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
       <c r="I189" s="3"/>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J189" s="5"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A190">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>189</v>
       </c>
       <c r="B190" s="3"/>
@@ -3369,10 +3607,11 @@
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
       <c r="I190" s="3"/>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J190" s="5"/>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A191">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
       <c r="B191" s="3"/>
@@ -3383,10 +3622,11 @@
       <c r="G191" s="3"/>
       <c r="H191" s="3"/>
       <c r="I191" s="3"/>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J191" s="5"/>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A192">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>191</v>
       </c>
       <c r="B192" s="3"/>
@@ -3397,10 +3637,11 @@
       <c r="G192" s="3"/>
       <c r="H192" s="3"/>
       <c r="I192" s="3"/>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J192" s="5"/>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A193">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="B193" s="3"/>
@@ -3411,10 +3652,11 @@
       <c r="G193" s="3"/>
       <c r="H193" s="3"/>
       <c r="I193" s="3"/>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J193" s="5"/>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A194">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" ref="A194:A251" si="3">ROW()-ROW(S_N)</f>
         <v>193</v>
       </c>
       <c r="B194" s="3"/>
@@ -3425,10 +3667,11 @@
       <c r="G194" s="3"/>
       <c r="H194" s="3"/>
       <c r="I194" s="3"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J194" s="5"/>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A195">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>194</v>
       </c>
       <c r="B195" s="3"/>
@@ -3439,10 +3682,11 @@
       <c r="G195" s="3"/>
       <c r="H195" s="3"/>
       <c r="I195" s="3"/>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J195" s="5"/>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A196">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>195</v>
       </c>
       <c r="B196" s="3"/>
@@ -3453,10 +3697,11 @@
       <c r="G196" s="3"/>
       <c r="H196" s="3"/>
       <c r="I196" s="3"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J196" s="5"/>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A197">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
       <c r="B197" s="3"/>
@@ -3467,10 +3712,11 @@
       <c r="G197" s="3"/>
       <c r="H197" s="3"/>
       <c r="I197" s="3"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J197" s="5"/>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A198">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>197</v>
       </c>
       <c r="B198" s="3"/>
@@ -3481,10 +3727,11 @@
       <c r="G198" s="3"/>
       <c r="H198" s="3"/>
       <c r="I198" s="3"/>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J198" s="5"/>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A199">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>198</v>
       </c>
       <c r="B199" s="3"/>
@@ -3495,10 +3742,11 @@
       <c r="G199" s="3"/>
       <c r="H199" s="3"/>
       <c r="I199" s="3"/>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J199" s="5"/>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A200">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>199</v>
       </c>
       <c r="B200" s="3"/>
@@ -3509,10 +3757,11 @@
       <c r="G200" s="3"/>
       <c r="H200" s="3"/>
       <c r="I200" s="3"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J200" s="5"/>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A201">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="B201" s="3"/>
@@ -3523,10 +3772,11 @@
       <c r="G201" s="3"/>
       <c r="H201" s="3"/>
       <c r="I201" s="3"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J201" s="5"/>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A202">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>201</v>
       </c>
       <c r="B202" s="3"/>
@@ -3537,10 +3787,11 @@
       <c r="G202" s="3"/>
       <c r="H202" s="3"/>
       <c r="I202" s="3"/>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J202" s="5"/>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A203">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>202</v>
       </c>
       <c r="B203" s="3"/>
@@ -3551,10 +3802,11 @@
       <c r="G203" s="3"/>
       <c r="H203" s="3"/>
       <c r="I203" s="3"/>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J203" s="5"/>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A204">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>203</v>
       </c>
       <c r="B204" s="3"/>
@@ -3565,10 +3817,11 @@
       <c r="G204" s="3"/>
       <c r="H204" s="3"/>
       <c r="I204" s="3"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J204" s="5"/>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A205">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>204</v>
       </c>
       <c r="B205" s="3"/>
@@ -3579,10 +3832,11 @@
       <c r="G205" s="3"/>
       <c r="H205" s="3"/>
       <c r="I205" s="3"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J205" s="5"/>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A206">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>205</v>
       </c>
       <c r="B206" s="3"/>
@@ -3593,10 +3847,11 @@
       <c r="G206" s="3"/>
       <c r="H206" s="3"/>
       <c r="I206" s="3"/>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J206" s="5"/>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A207">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>206</v>
       </c>
       <c r="B207" s="3"/>
@@ -3607,10 +3862,11 @@
       <c r="G207" s="3"/>
       <c r="H207" s="3"/>
       <c r="I207" s="3"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J207" s="5"/>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A208">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>207</v>
       </c>
       <c r="B208" s="3"/>
@@ -3621,10 +3877,11 @@
       <c r="G208" s="3"/>
       <c r="H208" s="3"/>
       <c r="I208" s="3"/>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J208" s="5"/>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A209">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="B209" s="3"/>
@@ -3635,10 +3892,11 @@
       <c r="G209" s="3"/>
       <c r="H209" s="3"/>
       <c r="I209" s="3"/>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J209" s="5"/>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A210">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>209</v>
       </c>
       <c r="B210" s="3"/>
@@ -3649,10 +3907,11 @@
       <c r="G210" s="3"/>
       <c r="H210" s="3"/>
       <c r="I210" s="3"/>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J210" s="5"/>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A211">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="B211" s="3"/>
@@ -3663,10 +3922,11 @@
       <c r="G211" s="3"/>
       <c r="H211" s="3"/>
       <c r="I211" s="3"/>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J211" s="5"/>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A212">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>211</v>
       </c>
       <c r="B212" s="3"/>
@@ -3677,10 +3937,11 @@
       <c r="G212" s="3"/>
       <c r="H212" s="3"/>
       <c r="I212" s="3"/>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J212" s="5"/>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A213">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>212</v>
       </c>
       <c r="B213" s="3"/>
@@ -3691,10 +3952,11 @@
       <c r="G213" s="3"/>
       <c r="H213" s="3"/>
       <c r="I213" s="3"/>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J213" s="5"/>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A214">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>213</v>
       </c>
       <c r="B214" s="3"/>
@@ -3705,10 +3967,11 @@
       <c r="G214" s="3"/>
       <c r="H214" s="3"/>
       <c r="I214" s="3"/>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J214" s="5"/>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A215">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>214</v>
       </c>
       <c r="B215" s="3"/>
@@ -3719,10 +3982,11 @@
       <c r="G215" s="3"/>
       <c r="H215" s="3"/>
       <c r="I215" s="3"/>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J215" s="5"/>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A216">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>215</v>
       </c>
       <c r="B216" s="3"/>
@@ -3733,10 +3997,11 @@
       <c r="G216" s="3"/>
       <c r="H216" s="3"/>
       <c r="I216" s="3"/>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J216" s="5"/>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A217">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>216</v>
       </c>
       <c r="B217" s="3"/>
@@ -3747,10 +4012,11 @@
       <c r="G217" s="3"/>
       <c r="H217" s="3"/>
       <c r="I217" s="3"/>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J217" s="5"/>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A218">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="B218" s="3"/>
@@ -3761,10 +4027,11 @@
       <c r="G218" s="3"/>
       <c r="H218" s="3"/>
       <c r="I218" s="3"/>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J218" s="5"/>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A219">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>218</v>
       </c>
       <c r="B219" s="3"/>
@@ -3775,10 +4042,11 @@
       <c r="G219" s="3"/>
       <c r="H219" s="3"/>
       <c r="I219" s="3"/>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J219" s="5"/>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A220">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>219</v>
       </c>
       <c r="B220" s="3"/>
@@ -3789,10 +4057,11 @@
       <c r="G220" s="3"/>
       <c r="H220" s="3"/>
       <c r="I220" s="3"/>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J220" s="5"/>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A221">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="B221" s="3"/>
@@ -3803,10 +4072,11 @@
       <c r="G221" s="3"/>
       <c r="H221" s="3"/>
       <c r="I221" s="3"/>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J221" s="5"/>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A222">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>221</v>
       </c>
       <c r="B222" s="3"/>
@@ -3817,10 +4087,11 @@
       <c r="G222" s="3"/>
       <c r="H222" s="3"/>
       <c r="I222" s="3"/>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J222" s="5"/>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A223">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>222</v>
       </c>
       <c r="B223" s="3"/>
@@ -3831,10 +4102,11 @@
       <c r="G223" s="3"/>
       <c r="H223" s="3"/>
       <c r="I223" s="3"/>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J223" s="5"/>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A224">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>223</v>
       </c>
       <c r="B224" s="3"/>
@@ -3845,10 +4117,11 @@
       <c r="G224" s="3"/>
       <c r="H224" s="3"/>
       <c r="I224" s="3"/>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J224" s="5"/>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A225">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>224</v>
       </c>
       <c r="B225" s="3"/>
@@ -3859,10 +4132,11 @@
       <c r="G225" s="3"/>
       <c r="H225" s="3"/>
       <c r="I225" s="3"/>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J225" s="5"/>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A226">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="B226" s="3"/>
@@ -3873,10 +4147,11 @@
       <c r="G226" s="3"/>
       <c r="H226" s="3"/>
       <c r="I226" s="3"/>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J226" s="5"/>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A227">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>226</v>
       </c>
       <c r="B227" s="3"/>
@@ -3887,10 +4162,11 @@
       <c r="G227" s="3"/>
       <c r="H227" s="3"/>
       <c r="I227" s="3"/>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J227" s="5"/>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A228">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>227</v>
       </c>
       <c r="B228" s="3"/>
@@ -3901,10 +4177,11 @@
       <c r="G228" s="3"/>
       <c r="H228" s="3"/>
       <c r="I228" s="3"/>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J228" s="5"/>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A229">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>228</v>
       </c>
       <c r="B229" s="3"/>
@@ -3915,10 +4192,11 @@
       <c r="G229" s="3"/>
       <c r="H229" s="3"/>
       <c r="I229" s="3"/>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J229" s="5"/>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A230">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>229</v>
       </c>
       <c r="B230" s="3"/>
@@ -3929,10 +4207,11 @@
       <c r="G230" s="3"/>
       <c r="H230" s="3"/>
       <c r="I230" s="3"/>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J230" s="5"/>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A231">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>230</v>
       </c>
       <c r="B231" s="3"/>
@@ -3943,10 +4222,11 @@
       <c r="G231" s="3"/>
       <c r="H231" s="3"/>
       <c r="I231" s="3"/>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J231" s="5"/>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A232">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>231</v>
       </c>
       <c r="B232" s="3"/>
@@ -3957,10 +4237,11 @@
       <c r="G232" s="3"/>
       <c r="H232" s="3"/>
       <c r="I232" s="3"/>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J232" s="5"/>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A233">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>232</v>
       </c>
       <c r="B233" s="3"/>
@@ -3971,10 +4252,11 @@
       <c r="G233" s="3"/>
       <c r="H233" s="3"/>
       <c r="I233" s="3"/>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J233" s="5"/>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A234">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>233</v>
       </c>
       <c r="B234" s="3"/>
@@ -3985,10 +4267,11 @@
       <c r="G234" s="3"/>
       <c r="H234" s="3"/>
       <c r="I234" s="3"/>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J234" s="5"/>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A235">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>234</v>
       </c>
       <c r="B235" s="3"/>
@@ -3999,10 +4282,11 @@
       <c r="G235" s="3"/>
       <c r="H235" s="3"/>
       <c r="I235" s="3"/>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J235" s="5"/>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A236">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>235</v>
       </c>
       <c r="B236" s="3"/>
@@ -4013,10 +4297,11 @@
       <c r="G236" s="3"/>
       <c r="H236" s="3"/>
       <c r="I236" s="3"/>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J236" s="5"/>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A237">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>236</v>
       </c>
       <c r="B237" s="3"/>
@@ -4027,10 +4312,11 @@
       <c r="G237" s="3"/>
       <c r="H237" s="3"/>
       <c r="I237" s="3"/>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J237" s="5"/>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A238">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>237</v>
       </c>
       <c r="B238" s="3"/>
@@ -4041,10 +4327,11 @@
       <c r="G238" s="3"/>
       <c r="H238" s="3"/>
       <c r="I238" s="3"/>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J238" s="5"/>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A239">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>238</v>
       </c>
       <c r="B239" s="3"/>
@@ -4055,10 +4342,11 @@
       <c r="G239" s="3"/>
       <c r="H239" s="3"/>
       <c r="I239" s="3"/>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J239" s="5"/>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A240">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>239</v>
       </c>
       <c r="B240" s="3"/>
@@ -4069,10 +4357,11 @@
       <c r="G240" s="3"/>
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J240" s="5"/>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A241">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="B241" s="3"/>
@@ -4083,10 +4372,11 @@
       <c r="G241" s="3"/>
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J241" s="5"/>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A242">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>241</v>
       </c>
       <c r="B242" s="3"/>
@@ -4097,10 +4387,11 @@
       <c r="G242" s="3"/>
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J242" s="5"/>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A243">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>242</v>
       </c>
       <c r="B243" s="3"/>
@@ -4111,10 +4402,11 @@
       <c r="G243" s="3"/>
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J243" s="5"/>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A244">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>243</v>
       </c>
       <c r="B244" s="3"/>
@@ -4125,10 +4417,11 @@
       <c r="G244" s="3"/>
       <c r="H244" s="3"/>
       <c r="I244" s="3"/>
-    </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J244" s="5"/>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A245">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>244</v>
       </c>
       <c r="B245" s="3"/>
@@ -4139,10 +4432,11 @@
       <c r="G245" s="3"/>
       <c r="H245" s="3"/>
       <c r="I245" s="3"/>
-    </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J245" s="5"/>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A246">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>245</v>
       </c>
       <c r="B246" s="3"/>
@@ -4153,10 +4447,11 @@
       <c r="G246" s="3"/>
       <c r="H246" s="3"/>
       <c r="I246" s="3"/>
-    </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J246" s="5"/>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A247">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>246</v>
       </c>
       <c r="B247" s="3"/>
@@ -4167,10 +4462,11 @@
       <c r="G247" s="3"/>
       <c r="H247" s="3"/>
       <c r="I247" s="3"/>
-    </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J247" s="5"/>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A248">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>247</v>
       </c>
       <c r="B248" s="3"/>
@@ -4181,10 +4477,11 @@
       <c r="G248" s="3"/>
       <c r="H248" s="3"/>
       <c r="I248" s="3"/>
-    </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J248" s="5"/>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A249">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>248</v>
       </c>
       <c r="B249" s="3"/>
@@ -4195,10 +4492,11 @@
       <c r="G249" s="3"/>
       <c r="H249" s="3"/>
       <c r="I249" s="3"/>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J249" s="5"/>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A250">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>249</v>
       </c>
       <c r="B250" s="3"/>
@@ -4209,10 +4507,11 @@
       <c r="G250" s="3"/>
       <c r="H250" s="3"/>
       <c r="I250" s="3"/>
-    </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J250" s="5"/>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A251">
-        <f>ROW()-ROW(S_N)</f>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="B251" s="4"/>
@@ -4223,10 +4522,11 @@
       <c r="G251" s="4"/>
       <c r="H251" s="4"/>
       <c r="I251" s="4"/>
-    </row>
-    <row r="253" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.65"/>
+      <c r="J251" s="5"/>
+    </row>
+    <row r="253" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.65"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Remove missed sessions from spreadsheet
</commit_message>
<xml_diff>
--- a/static/excel/samples/student_bio_data.xlsx
+++ b/static/excel/samples/student_bio_data.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39146C02-D176-48AF-8B95-482C1F5B62B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1708135-0D28-4CD8-BA63-8231497DD9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="S_N" localSheetId="0">Sheet1!$A$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,13 +61,19 @@
     <t>Single</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
     <t>S/N</t>
+  </si>
+  <si>
+    <t>Rivers</t>
+  </si>
+  <si>
+    <t>Missed Sessions</t>
+  </si>
+  <si>
+    <t>U2015/3025100</t>
   </si>
   <si>
     <t>Jane</t>
@@ -79,16 +82,10 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>U2015/3025000</t>
+    <t>F</t>
   </si>
   <si>
-    <t>Rivers</t>
-  </si>
-  <si>
-    <t>Missed Sessions</t>
-  </si>
-  <si>
-    <t>2015/2016, 2016/2017, 2017/2018</t>
+    <t>2018/2019, 2019/2020</t>
   </si>
 </sst>
 </file>
@@ -211,6 +208,14 @@
     <cellStyle name="Number Style" xfId="1" xr:uid="{3F35957B-008B-4DD5-888E-1BF85505A66E}"/>
   </cellStyles>
   <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -336,13 +341,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -426,18 +424,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7BAF8AF9-FE7E-4C26-9CE5-39B51F7A0A6F}" name="Table3" displayName="Table3" ref="A1:J251" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{03666201-703C-4511-955E-41CFD2A5964C}" name="S/N" dataDxfId="9">
-      <calculatedColumnFormula>ROW()-ROW(S_N)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{03666201-703C-4511-955E-41CFD2A5964C}" name="S/N" dataDxfId="0">
+      <calculatedColumnFormula>ROW()-ROW(Table3[[#Headers],[S/N]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A4F45E95-3E87-4B8D-948D-CBC14E8BE626}" name="Matric NO" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{5654AEB4-E02D-46F2-9097-268CC0AA5555}" name="First Name" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{4B079751-EAF1-4002-9342-AB8C668AED98}" name="Last Name" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{610752AC-CE04-44A9-8522-7A50EA38594A}" name="Other Names" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{8DA555E0-9C62-4F9F-A965-3CAC2E10D1B3}" name="Department" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{0543A9BF-C2F0-4261-A622-B5F2375F163E}" name="Sex" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{56AF198A-6CBE-4431-A8D6-7600C3EF332C}" name="State of Origin" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{659CEECD-EEAE-4A20-B4C0-9A931DA6805B}" name="Marital Status" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{BF72F716-1468-45D7-867F-EC38F8392790}" name="Missed Sessions" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{A4F45E95-3E87-4B8D-948D-CBC14E8BE626}" name="Matric NO" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5654AEB4-E02D-46F2-9097-268CC0AA5555}" name="First Name" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4B079751-EAF1-4002-9342-AB8C668AED98}" name="Last Name" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{610752AC-CE04-44A9-8522-7A50EA38594A}" name="Other Names" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{8DA555E0-9C62-4F9F-A965-3CAC2E10D1B3}" name="Department" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{0543A9BF-C2F0-4261-A622-B5F2375F163E}" name="Sex" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{56AF198A-6CBE-4431-A8D6-7600C3EF332C}" name="State of Origin" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{659CEECD-EEAE-4A20-B4C0-9A931DA6805B}" name="Marital Status" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{BF72F716-1468-45D7-867F-EC38F8392790}" name="Missed Sessions" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Semester Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,9 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -728,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -743,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -755,32 +751,32 @@
         <v>6</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2">
-        <f t="shared" ref="A2:A65" si="0">ROW()-ROW(S_N)</f>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
@@ -791,7 +787,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
@@ -806,7 +802,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
@@ -821,7 +817,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
@@ -836,7 +832,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>5</v>
       </c>
       <c r="B6" s="3"/>
@@ -851,7 +847,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
@@ -866,7 +862,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
@@ -881,7 +877,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
@@ -896,7 +892,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
@@ -911,7 +907,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>10</v>
       </c>
       <c r="B11" s="3"/>
@@ -926,7 +922,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>11</v>
       </c>
       <c r="B12" s="3"/>
@@ -941,7 +937,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>12</v>
       </c>
       <c r="B13" s="3"/>
@@ -956,7 +952,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
@@ -971,7 +967,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
@@ -986,7 +982,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>15</v>
       </c>
       <c r="B16" s="3"/>
@@ -1001,7 +997,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>16</v>
       </c>
       <c r="B17" s="3"/>
@@ -1016,7 +1012,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>17</v>
       </c>
       <c r="B18" s="3"/>
@@ -1031,7 +1027,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>18</v>
       </c>
       <c r="B19" s="3"/>
@@ -1046,7 +1042,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>19</v>
       </c>
       <c r="B20" s="3"/>
@@ -1061,7 +1057,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>20</v>
       </c>
       <c r="B21" s="3"/>
@@ -1076,7 +1072,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>21</v>
       </c>
       <c r="B22" s="3"/>
@@ -1091,7 +1087,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>22</v>
       </c>
       <c r="B23" s="3"/>
@@ -1106,7 +1102,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>23</v>
       </c>
       <c r="B24" s="3"/>
@@ -1121,7 +1117,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>24</v>
       </c>
       <c r="B25" s="3"/>
@@ -1136,7 +1132,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>25</v>
       </c>
       <c r="B26" s="3"/>
@@ -1151,7 +1147,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>26</v>
       </c>
       <c r="B27" s="3"/>
@@ -1166,7 +1162,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>27</v>
       </c>
       <c r="B28" s="3"/>
@@ -1181,7 +1177,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>28</v>
       </c>
       <c r="B29" s="3"/>
@@ -1196,7 +1192,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>29</v>
       </c>
       <c r="B30" s="3"/>
@@ -1211,7 +1207,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>30</v>
       </c>
       <c r="B31" s="3"/>
@@ -1226,7 +1222,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>31</v>
       </c>
       <c r="B32" s="3"/>
@@ -1241,7 +1237,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>32</v>
       </c>
       <c r="B33" s="3"/>
@@ -1256,7 +1252,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>33</v>
       </c>
       <c r="B34" s="3"/>
@@ -1271,7 +1267,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>34</v>
       </c>
       <c r="B35" s="3"/>
@@ -1286,7 +1282,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>35</v>
       </c>
       <c r="B36" s="3"/>
@@ -1301,7 +1297,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>36</v>
       </c>
       <c r="B37" s="3"/>
@@ -1316,7 +1312,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>37</v>
       </c>
       <c r="B38" s="3"/>
@@ -1331,7 +1327,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>38</v>
       </c>
       <c r="B39" s="3"/>
@@ -1346,7 +1342,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>39</v>
       </c>
       <c r="B40" s="3"/>
@@ -1361,7 +1357,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>40</v>
       </c>
       <c r="B41" s="3"/>
@@ -1376,7 +1372,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>41</v>
       </c>
       <c r="B42" s="3"/>
@@ -1391,7 +1387,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>42</v>
       </c>
       <c r="B43" s="3"/>
@@ -1406,7 +1402,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>43</v>
       </c>
       <c r="B44" s="3"/>
@@ -1421,7 +1417,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>44</v>
       </c>
       <c r="B45" s="3"/>
@@ -1436,7 +1432,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>45</v>
       </c>
       <c r="B46" s="3"/>
@@ -1451,7 +1447,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>46</v>
       </c>
       <c r="B47" s="3"/>
@@ -1466,7 +1462,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>47</v>
       </c>
       <c r="B48" s="3"/>
@@ -1481,7 +1477,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>48</v>
       </c>
       <c r="B49" s="3"/>
@@ -1496,7 +1492,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>49</v>
       </c>
       <c r="B50" s="3"/>
@@ -1511,7 +1507,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>50</v>
       </c>
       <c r="B51" s="3"/>
@@ -1526,7 +1522,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>51</v>
       </c>
       <c r="B52" s="3"/>
@@ -1541,7 +1537,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>52</v>
       </c>
       <c r="B53" s="3"/>
@@ -1556,7 +1552,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>53</v>
       </c>
       <c r="B54" s="3"/>
@@ -1571,7 +1567,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>54</v>
       </c>
       <c r="B55" s="3"/>
@@ -1586,7 +1582,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>55</v>
       </c>
       <c r="B56" s="3"/>
@@ -1601,7 +1597,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>56</v>
       </c>
       <c r="B57" s="3"/>
@@ -1616,7 +1612,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>57</v>
       </c>
       <c r="B58" s="3"/>
@@ -1631,7 +1627,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>58</v>
       </c>
       <c r="B59" s="3"/>
@@ -1646,7 +1642,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>59</v>
       </c>
       <c r="B60" s="3"/>
@@ -1661,7 +1657,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A61">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>60</v>
       </c>
       <c r="B61" s="3"/>
@@ -1676,7 +1672,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A62">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>61</v>
       </c>
       <c r="B62" s="3"/>
@@ -1691,7 +1687,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A63">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>62</v>
       </c>
       <c r="B63" s="3"/>
@@ -1706,7 +1702,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A64">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>63</v>
       </c>
       <c r="B64" s="3"/>
@@ -1721,7 +1717,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A65">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>64</v>
       </c>
       <c r="B65" s="3"/>
@@ -1736,7 +1732,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A66">
-        <f t="shared" ref="A66:A129" si="1">ROW()-ROW(S_N)</f>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>65</v>
       </c>
       <c r="B66" s="3"/>
@@ -1751,7 +1747,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A67">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>66</v>
       </c>
       <c r="B67" s="3"/>
@@ -1766,7 +1762,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A68">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>67</v>
       </c>
       <c r="B68" s="3"/>
@@ -1781,7 +1777,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A69">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>68</v>
       </c>
       <c r="B69" s="3"/>
@@ -1796,7 +1792,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A70">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>69</v>
       </c>
       <c r="B70" s="3"/>
@@ -1811,7 +1807,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A71">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>70</v>
       </c>
       <c r="B71" s="3"/>
@@ -1826,7 +1822,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A72">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>71</v>
       </c>
       <c r="B72" s="3"/>
@@ -1841,7 +1837,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A73">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>72</v>
       </c>
       <c r="B73" s="3"/>
@@ -1856,7 +1852,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A74">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>73</v>
       </c>
       <c r="B74" s="3"/>
@@ -1871,7 +1867,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A75">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>74</v>
       </c>
       <c r="B75" s="3"/>
@@ -1886,7 +1882,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A76">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>75</v>
       </c>
       <c r="B76" s="3"/>
@@ -1901,7 +1897,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A77">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>76</v>
       </c>
       <c r="B77" s="3"/>
@@ -1916,7 +1912,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A78">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>77</v>
       </c>
       <c r="B78" s="3"/>
@@ -1931,7 +1927,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A79">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>78</v>
       </c>
       <c r="B79" s="3"/>
@@ -1946,7 +1942,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A80">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>79</v>
       </c>
       <c r="B80" s="3"/>
@@ -1961,7 +1957,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A81">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>80</v>
       </c>
       <c r="B81" s="3"/>
@@ -1976,7 +1972,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A82">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>81</v>
       </c>
       <c r="B82" s="3"/>
@@ -1991,7 +1987,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A83">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>82</v>
       </c>
       <c r="B83" s="3"/>
@@ -2006,7 +2002,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A84">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>83</v>
       </c>
       <c r="B84" s="3"/>
@@ -2021,7 +2017,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A85">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>84</v>
       </c>
       <c r="B85" s="3"/>
@@ -2036,7 +2032,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A86">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>85</v>
       </c>
       <c r="B86" s="3"/>
@@ -2051,7 +2047,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A87">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>86</v>
       </c>
       <c r="B87" s="3"/>
@@ -2066,7 +2062,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A88">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>87</v>
       </c>
       <c r="B88" s="3"/>
@@ -2081,7 +2077,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A89">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>88</v>
       </c>
       <c r="B89" s="3"/>
@@ -2096,7 +2092,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A90">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>89</v>
       </c>
       <c r="B90" s="3"/>
@@ -2111,7 +2107,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A91">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>90</v>
       </c>
       <c r="B91" s="3"/>
@@ -2126,7 +2122,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A92">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>91</v>
       </c>
       <c r="B92" s="3"/>
@@ -2141,7 +2137,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A93">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>92</v>
       </c>
       <c r="B93" s="3"/>
@@ -2156,7 +2152,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A94">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>93</v>
       </c>
       <c r="B94" s="3"/>
@@ -2171,7 +2167,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A95">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>94</v>
       </c>
       <c r="B95" s="3"/>
@@ -2186,7 +2182,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A96">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>95</v>
       </c>
       <c r="B96" s="3"/>
@@ -2201,7 +2197,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A97">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>96</v>
       </c>
       <c r="B97" s="3"/>
@@ -2216,7 +2212,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A98">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>97</v>
       </c>
       <c r="B98" s="3"/>
@@ -2231,7 +2227,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A99">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>98</v>
       </c>
       <c r="B99" s="3"/>
@@ -2246,7 +2242,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A100">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>99</v>
       </c>
       <c r="B100" s="3"/>
@@ -2261,7 +2257,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A101">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>100</v>
       </c>
       <c r="B101" s="3"/>
@@ -2276,7 +2272,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A102">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>101</v>
       </c>
       <c r="B102" s="3"/>
@@ -2291,7 +2287,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A103">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>102</v>
       </c>
       <c r="B103" s="3"/>
@@ -2306,7 +2302,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A104">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>103</v>
       </c>
       <c r="B104" s="3"/>
@@ -2321,7 +2317,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A105">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>104</v>
       </c>
       <c r="B105" s="3"/>
@@ -2336,7 +2332,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A106">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>105</v>
       </c>
       <c r="B106" s="3"/>
@@ -2351,7 +2347,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A107">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>106</v>
       </c>
       <c r="B107" s="3"/>
@@ -2366,7 +2362,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A108">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>107</v>
       </c>
       <c r="B108" s="3"/>
@@ -2381,7 +2377,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A109">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>108</v>
       </c>
       <c r="B109" s="3"/>
@@ -2396,7 +2392,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A110">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>109</v>
       </c>
       <c r="B110" s="3"/>
@@ -2411,7 +2407,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A111">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>110</v>
       </c>
       <c r="B111" s="3"/>
@@ -2426,7 +2422,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A112">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>111</v>
       </c>
       <c r="B112" s="3"/>
@@ -2441,7 +2437,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A113">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>112</v>
       </c>
       <c r="B113" s="3"/>
@@ -2456,7 +2452,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A114">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>113</v>
       </c>
       <c r="B114" s="3"/>
@@ -2471,7 +2467,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A115">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>114</v>
       </c>
       <c r="B115" s="3"/>
@@ -2486,7 +2482,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A116">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>115</v>
       </c>
       <c r="B116" s="3"/>
@@ -2501,7 +2497,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A117">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>116</v>
       </c>
       <c r="B117" s="3"/>
@@ -2516,7 +2512,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A118">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>117</v>
       </c>
       <c r="B118" s="3"/>
@@ -2531,7 +2527,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A119">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>118</v>
       </c>
       <c r="B119" s="3"/>
@@ -2546,7 +2542,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A120">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>119</v>
       </c>
       <c r="B120" s="3"/>
@@ -2561,7 +2557,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A121">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>120</v>
       </c>
       <c r="B121" s="3"/>
@@ -2576,7 +2572,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A122">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>121</v>
       </c>
       <c r="B122" s="3"/>
@@ -2591,7 +2587,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A123">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>122</v>
       </c>
       <c r="B123" s="3"/>
@@ -2606,7 +2602,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A124">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>123</v>
       </c>
       <c r="B124" s="3"/>
@@ -2621,7 +2617,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A125">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>124</v>
       </c>
       <c r="B125" s="3"/>
@@ -2636,7 +2632,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A126">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>125</v>
       </c>
       <c r="B126" s="3"/>
@@ -2651,7 +2647,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A127">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>126</v>
       </c>
       <c r="B127" s="3"/>
@@ -2666,7 +2662,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A128">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>127</v>
       </c>
       <c r="B128" s="3"/>
@@ -2681,7 +2677,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A129">
-        <f t="shared" si="1"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>128</v>
       </c>
       <c r="B129" s="3"/>
@@ -2696,7 +2692,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A130">
-        <f t="shared" ref="A130:A193" si="2">ROW()-ROW(S_N)</f>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>129</v>
       </c>
       <c r="B130" s="3"/>
@@ -2711,7 +2707,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A131">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>130</v>
       </c>
       <c r="B131" s="3"/>
@@ -2726,7 +2722,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A132">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>131</v>
       </c>
       <c r="B132" s="3"/>
@@ -2741,7 +2737,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A133">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>132</v>
       </c>
       <c r="B133" s="3"/>
@@ -2756,7 +2752,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A134">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>133</v>
       </c>
       <c r="B134" s="3"/>
@@ -2771,7 +2767,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A135">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>134</v>
       </c>
       <c r="B135" s="3"/>
@@ -2786,7 +2782,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A136">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>135</v>
       </c>
       <c r="B136" s="3"/>
@@ -2801,7 +2797,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A137">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>136</v>
       </c>
       <c r="B137" s="3"/>
@@ -2816,7 +2812,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A138">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>137</v>
       </c>
       <c r="B138" s="3"/>
@@ -2831,7 +2827,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A139">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>138</v>
       </c>
       <c r="B139" s="3"/>
@@ -2846,7 +2842,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A140">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>139</v>
       </c>
       <c r="B140" s="3"/>
@@ -2861,7 +2857,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A141">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>140</v>
       </c>
       <c r="B141" s="3"/>
@@ -2876,7 +2872,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A142">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>141</v>
       </c>
       <c r="B142" s="3"/>
@@ -2891,7 +2887,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A143">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>142</v>
       </c>
       <c r="B143" s="3"/>
@@ -2906,7 +2902,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A144">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>143</v>
       </c>
       <c r="B144" s="3"/>
@@ -2921,7 +2917,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A145">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>144</v>
       </c>
       <c r="B145" s="3"/>
@@ -2936,7 +2932,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A146">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>145</v>
       </c>
       <c r="B146" s="3"/>
@@ -2951,7 +2947,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A147">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>146</v>
       </c>
       <c r="B147" s="3"/>
@@ -2966,7 +2962,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A148">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>147</v>
       </c>
       <c r="B148" s="3"/>
@@ -2981,7 +2977,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A149">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>148</v>
       </c>
       <c r="B149" s="3"/>
@@ -2996,7 +2992,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A150">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>149</v>
       </c>
       <c r="B150" s="3"/>
@@ -3011,7 +3007,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A151">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>150</v>
       </c>
       <c r="B151" s="3"/>
@@ -3026,7 +3022,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A152">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>151</v>
       </c>
       <c r="B152" s="3"/>
@@ -3041,7 +3037,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A153">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>152</v>
       </c>
       <c r="B153" s="3"/>
@@ -3056,7 +3052,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A154">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>153</v>
       </c>
       <c r="B154" s="3"/>
@@ -3071,7 +3067,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A155">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>154</v>
       </c>
       <c r="B155" s="3"/>
@@ -3086,7 +3082,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A156">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>155</v>
       </c>
       <c r="B156" s="3"/>
@@ -3101,7 +3097,7 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A157">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>156</v>
       </c>
       <c r="B157" s="3"/>
@@ -3116,7 +3112,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A158">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>157</v>
       </c>
       <c r="B158" s="3"/>
@@ -3131,7 +3127,7 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A159">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>158</v>
       </c>
       <c r="B159" s="3"/>
@@ -3146,7 +3142,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A160">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>159</v>
       </c>
       <c r="B160" s="3"/>
@@ -3161,7 +3157,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A161">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>160</v>
       </c>
       <c r="B161" s="3"/>
@@ -3176,7 +3172,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A162">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>161</v>
       </c>
       <c r="B162" s="3"/>
@@ -3191,7 +3187,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A163">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>162</v>
       </c>
       <c r="B163" s="3"/>
@@ -3206,7 +3202,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A164">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>163</v>
       </c>
       <c r="B164" s="3"/>
@@ -3221,7 +3217,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A165">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>164</v>
       </c>
       <c r="B165" s="3"/>
@@ -3236,7 +3232,7 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A166">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>165</v>
       </c>
       <c r="B166" s="3"/>
@@ -3251,7 +3247,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A167">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>166</v>
       </c>
       <c r="B167" s="3"/>
@@ -3266,7 +3262,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A168">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>167</v>
       </c>
       <c r="B168" s="3"/>
@@ -3281,7 +3277,7 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A169">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>168</v>
       </c>
       <c r="B169" s="3"/>
@@ -3296,7 +3292,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A170">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>169</v>
       </c>
       <c r="B170" s="3"/>
@@ -3311,7 +3307,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A171">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>170</v>
       </c>
       <c r="B171" s="3"/>
@@ -3326,7 +3322,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A172">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>171</v>
       </c>
       <c r="B172" s="3"/>
@@ -3341,7 +3337,7 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A173">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>172</v>
       </c>
       <c r="B173" s="3"/>
@@ -3356,7 +3352,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A174">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>173</v>
       </c>
       <c r="B174" s="3"/>
@@ -3371,7 +3367,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A175">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>174</v>
       </c>
       <c r="B175" s="3"/>
@@ -3386,7 +3382,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A176">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>175</v>
       </c>
       <c r="B176" s="3"/>
@@ -3401,7 +3397,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A177">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>176</v>
       </c>
       <c r="B177" s="3"/>
@@ -3416,7 +3412,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A178">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>177</v>
       </c>
       <c r="B178" s="3"/>
@@ -3431,7 +3427,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A179">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>178</v>
       </c>
       <c r="B179" s="3"/>
@@ -3446,7 +3442,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A180">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>179</v>
       </c>
       <c r="B180" s="3"/>
@@ -3461,7 +3457,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A181">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>180</v>
       </c>
       <c r="B181" s="3"/>
@@ -3476,7 +3472,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A182">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>181</v>
       </c>
       <c r="B182" s="3"/>
@@ -3491,7 +3487,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A183">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>182</v>
       </c>
       <c r="B183" s="3"/>
@@ -3506,7 +3502,7 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A184">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>183</v>
       </c>
       <c r="B184" s="3"/>
@@ -3521,7 +3517,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A185">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>184</v>
       </c>
       <c r="B185" s="3"/>
@@ -3536,7 +3532,7 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A186">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>185</v>
       </c>
       <c r="B186" s="3"/>
@@ -3551,7 +3547,7 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A187">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>186</v>
       </c>
       <c r="B187" s="3"/>
@@ -3566,7 +3562,7 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A188">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>187</v>
       </c>
       <c r="B188" s="3"/>
@@ -3581,7 +3577,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A189">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>188</v>
       </c>
       <c r="B189" s="3"/>
@@ -3596,7 +3592,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A190">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>189</v>
       </c>
       <c r="B190" s="3"/>
@@ -3611,7 +3607,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A191">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>190</v>
       </c>
       <c r="B191" s="3"/>
@@ -3626,7 +3622,7 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A192">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>191</v>
       </c>
       <c r="B192" s="3"/>
@@ -3641,7 +3637,7 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A193">
-        <f t="shared" si="2"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>192</v>
       </c>
       <c r="B193" s="3"/>
@@ -3656,7 +3652,7 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A194">
-        <f t="shared" ref="A194:A251" si="3">ROW()-ROW(S_N)</f>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>193</v>
       </c>
       <c r="B194" s="3"/>
@@ -3671,7 +3667,7 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A195">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>194</v>
       </c>
       <c r="B195" s="3"/>
@@ -3686,7 +3682,7 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A196">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>195</v>
       </c>
       <c r="B196" s="3"/>
@@ -3701,7 +3697,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A197">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>196</v>
       </c>
       <c r="B197" s="3"/>
@@ -3716,7 +3712,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A198">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>197</v>
       </c>
       <c r="B198" s="3"/>
@@ -3731,7 +3727,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A199">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>198</v>
       </c>
       <c r="B199" s="3"/>
@@ -3746,7 +3742,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A200">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>199</v>
       </c>
       <c r="B200" s="3"/>
@@ -3761,7 +3757,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A201">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>200</v>
       </c>
       <c r="B201" s="3"/>
@@ -3776,7 +3772,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A202">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>201</v>
       </c>
       <c r="B202" s="3"/>
@@ -3791,7 +3787,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A203">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>202</v>
       </c>
       <c r="B203" s="3"/>
@@ -3806,7 +3802,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A204">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>203</v>
       </c>
       <c r="B204" s="3"/>
@@ -3821,7 +3817,7 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A205">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>204</v>
       </c>
       <c r="B205" s="3"/>
@@ -3836,7 +3832,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A206">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>205</v>
       </c>
       <c r="B206" s="3"/>
@@ -3851,7 +3847,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A207">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>206</v>
       </c>
       <c r="B207" s="3"/>
@@ -3866,7 +3862,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A208">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>207</v>
       </c>
       <c r="B208" s="3"/>
@@ -3881,7 +3877,7 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A209">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>208</v>
       </c>
       <c r="B209" s="3"/>
@@ -3896,7 +3892,7 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A210">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>209</v>
       </c>
       <c r="B210" s="3"/>
@@ -3911,7 +3907,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A211">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>210</v>
       </c>
       <c r="B211" s="3"/>
@@ -3926,7 +3922,7 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A212">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>211</v>
       </c>
       <c r="B212" s="3"/>
@@ -3941,7 +3937,7 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A213">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>212</v>
       </c>
       <c r="B213" s="3"/>
@@ -3956,7 +3952,7 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A214">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>213</v>
       </c>
       <c r="B214" s="3"/>
@@ -3971,7 +3967,7 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A215">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>214</v>
       </c>
       <c r="B215" s="3"/>
@@ -3986,7 +3982,7 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A216">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>215</v>
       </c>
       <c r="B216" s="3"/>
@@ -4001,7 +3997,7 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A217">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>216</v>
       </c>
       <c r="B217" s="3"/>
@@ -4016,7 +4012,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A218">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>217</v>
       </c>
       <c r="B218" s="3"/>
@@ -4031,7 +4027,7 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A219">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>218</v>
       </c>
       <c r="B219" s="3"/>
@@ -4046,7 +4042,7 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A220">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>219</v>
       </c>
       <c r="B220" s="3"/>
@@ -4061,7 +4057,7 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A221">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>220</v>
       </c>
       <c r="B221" s="3"/>
@@ -4076,7 +4072,7 @@
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A222">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>221</v>
       </c>
       <c r="B222" s="3"/>
@@ -4091,7 +4087,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A223">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>222</v>
       </c>
       <c r="B223" s="3"/>
@@ -4106,7 +4102,7 @@
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A224">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>223</v>
       </c>
       <c r="B224" s="3"/>
@@ -4121,7 +4117,7 @@
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A225">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>224</v>
       </c>
       <c r="B225" s="3"/>
@@ -4136,7 +4132,7 @@
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A226">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>225</v>
       </c>
       <c r="B226" s="3"/>
@@ -4151,7 +4147,7 @@
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A227">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>226</v>
       </c>
       <c r="B227" s="3"/>
@@ -4166,7 +4162,7 @@
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A228">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>227</v>
       </c>
       <c r="B228" s="3"/>
@@ -4181,7 +4177,7 @@
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A229">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>228</v>
       </c>
       <c r="B229" s="3"/>
@@ -4196,7 +4192,7 @@
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A230">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>229</v>
       </c>
       <c r="B230" s="3"/>
@@ -4211,7 +4207,7 @@
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A231">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>230</v>
       </c>
       <c r="B231" s="3"/>
@@ -4226,7 +4222,7 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A232">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>231</v>
       </c>
       <c r="B232" s="3"/>
@@ -4241,7 +4237,7 @@
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A233">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>232</v>
       </c>
       <c r="B233" s="3"/>
@@ -4256,7 +4252,7 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A234">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>233</v>
       </c>
       <c r="B234" s="3"/>
@@ -4271,7 +4267,7 @@
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A235">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>234</v>
       </c>
       <c r="B235" s="3"/>
@@ -4286,7 +4282,7 @@
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A236">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>235</v>
       </c>
       <c r="B236" s="3"/>
@@ -4301,7 +4297,7 @@
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A237">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>236</v>
       </c>
       <c r="B237" s="3"/>
@@ -4316,7 +4312,7 @@
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A238">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>237</v>
       </c>
       <c r="B238" s="3"/>
@@ -4331,7 +4327,7 @@
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A239">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>238</v>
       </c>
       <c r="B239" s="3"/>
@@ -4346,7 +4342,7 @@
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A240">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>239</v>
       </c>
       <c r="B240" s="3"/>
@@ -4361,7 +4357,7 @@
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A241">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>240</v>
       </c>
       <c r="B241" s="3"/>
@@ -4376,7 +4372,7 @@
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A242">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>241</v>
       </c>
       <c r="B242" s="3"/>
@@ -4391,7 +4387,7 @@
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A243">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>242</v>
       </c>
       <c r="B243" s="3"/>
@@ -4406,7 +4402,7 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A244">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>243</v>
       </c>
       <c r="B244" s="3"/>
@@ -4421,7 +4417,7 @@
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A245">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>244</v>
       </c>
       <c r="B245" s="3"/>
@@ -4436,7 +4432,7 @@
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A246">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>245</v>
       </c>
       <c r="B246" s="3"/>
@@ -4451,7 +4447,7 @@
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A247">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>246</v>
       </c>
       <c r="B247" s="3"/>
@@ -4466,7 +4462,7 @@
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A248">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>247</v>
       </c>
       <c r="B248" s="3"/>
@@ -4481,7 +4477,7 @@
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A249">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>248</v>
       </c>
       <c r="B249" s="3"/>
@@ -4496,7 +4492,7 @@
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A250">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>249</v>
       </c>
       <c r="B250" s="3"/>
@@ -4511,7 +4507,7 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A251">
-        <f t="shared" si="3"/>
+        <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>250</v>
       </c>
       <c r="B251" s="4"/>

</xml_diff>

<commit_message>
feat: add graduation to summary
</commit_message>
<xml_diff>
--- a/static/excel/samples/student_bio_data.xlsx
+++ b/static/excel/samples/student_bio_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1708135-0D28-4CD8-BA63-8231497DD9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45194337-FA0A-4F85-9363-DDB6919D62D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Matric NO</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>2018/2019, 2019/2020</t>
+  </si>
+  <si>
+    <t>Graduate</t>
   </si>
 </sst>
 </file>
@@ -207,14 +210,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number Style" xfId="1" xr:uid="{3F35957B-008B-4DD5-888E-1BF85505A66E}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -334,6 +342,14 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <right style="thin">
           <color auto="1"/>
@@ -405,9 +421,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Semester Style" pivot="0" count="3" xr9:uid="{76CBB96B-0C45-4CF6-A9BA-2FA186E32BFA}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="totalRow" dxfId="13"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -422,9 +438,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7BAF8AF9-FE7E-4C26-9CE5-39B51F7A0A6F}" name="Table3" displayName="Table3" ref="A1:J251" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{03666201-703C-4511-955E-41CFD2A5964C}" name="S/N" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7BAF8AF9-FE7E-4C26-9CE5-39B51F7A0A6F}" name="Table3" displayName="Table3" ref="A1:K251" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{03666201-703C-4511-955E-41CFD2A5964C}" name="S/N" dataDxfId="10">
       <calculatedColumnFormula>ROW()-ROW(Table3[[#Headers],[S/N]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{A4F45E95-3E87-4B8D-948D-CBC14E8BE626}" name="Matric NO" dataDxfId="9"/>
@@ -436,6 +452,7 @@
     <tableColumn id="8" xr3:uid="{56AF198A-6CBE-4431-A8D6-7600C3EF332C}" name="State of Origin" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{659CEECD-EEAE-4A20-B4C0-9A931DA6805B}" name="Marital Status" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{BF72F716-1468-45D7-867F-EC38F8392790}" name="Missed Sessions" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{4A201ACE-417C-491A-8E2D-FF5EB8C0C693}" name="Graduate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Semester Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -704,25 +721,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J253"/>
+  <dimension ref="A1:K253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.58984375" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.58984375" customWidth="1"/>
-    <col min="4" max="4" width="11.31640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="15.2265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.40625" customWidth="1"/>
-    <col min="8" max="8" width="14.6328125" customWidth="1"/>
-    <col min="9" max="9" width="14.36328125" customWidth="1"/>
-    <col min="10" max="10" width="32.453125" customWidth="1"/>
+    <col min="1" max="1" width="5.578125" customWidth="1"/>
+    <col min="2" max="2" width="15.26171875" customWidth="1"/>
+    <col min="3" max="3" width="11.578125" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" customWidth="1"/>
+    <col min="5" max="5" width="13.62890625" customWidth="1"/>
+    <col min="6" max="6" width="15.20703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.41796875" customWidth="1"/>
+    <col min="8" max="8" width="14.62890625" customWidth="1"/>
+    <col min="9" max="9" width="14.3671875" customWidth="1"/>
+    <col min="10" max="10" width="26.734375" customWidth="1"/>
+    <col min="11" max="11" width="15.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -753,8 +773,11 @@
       <c r="J1" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>1</v>
@@ -784,8 +807,11 @@
       <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K2" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>2</v>
@@ -799,8 +825,9 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>3</v>
@@ -814,8 +841,9 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>4</v>
@@ -829,8 +857,9 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>5</v>
@@ -844,8 +873,9 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>6</v>
@@ -859,8 +889,9 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>7</v>
@@ -874,8 +905,9 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>8</v>
@@ -889,8 +921,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>9</v>
@@ -904,8 +937,9 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>10</v>
@@ -919,8 +953,9 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>11</v>
@@ -934,8 +969,9 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>12</v>
@@ -949,8 +985,9 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>13</v>
@@ -964,8 +1001,9 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>14</v>
@@ -979,8 +1017,9 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>15</v>
@@ -994,8 +1033,9 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>16</v>
@@ -1009,8 +1049,9 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>17</v>
@@ -1024,8 +1065,9 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>18</v>
@@ -1039,8 +1081,9 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>19</v>
@@ -1054,8 +1097,9 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>20</v>
@@ -1069,8 +1113,9 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>21</v>
@@ -1084,8 +1129,9 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>22</v>
@@ -1099,8 +1145,9 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>23</v>
@@ -1114,8 +1161,9 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>24</v>
@@ -1129,8 +1177,9 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>25</v>
@@ -1144,8 +1193,9 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>26</v>
@@ -1159,8 +1209,9 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>27</v>
@@ -1174,8 +1225,9 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>28</v>
@@ -1189,8 +1241,9 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>29</v>
@@ -1204,8 +1257,9 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>30</v>
@@ -1219,8 +1273,9 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>31</v>
@@ -1234,8 +1289,9 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>32</v>
@@ -1249,8 +1305,9 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>33</v>
@@ -1264,8 +1321,9 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>34</v>
@@ -1279,8 +1337,9 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>35</v>
@@ -1294,8 +1353,9 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>36</v>
@@ -1309,8 +1369,9 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>37</v>
@@ -1324,8 +1385,9 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>38</v>
@@ -1339,8 +1401,9 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>39</v>
@@ -1354,8 +1417,9 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>40</v>
@@ -1369,8 +1433,9 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>41</v>
@@ -1384,8 +1449,9 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>42</v>
@@ -1399,8 +1465,9 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>43</v>
@@ -1414,8 +1481,9 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>44</v>
@@ -1429,8 +1497,9 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>45</v>
@@ -1444,8 +1513,9 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>46</v>
@@ -1459,8 +1529,9 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>47</v>
@@ -1474,8 +1545,9 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>48</v>
@@ -1489,8 +1561,9 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>49</v>
@@ -1504,8 +1577,9 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>50</v>
@@ -1519,8 +1593,9 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>51</v>
@@ -1534,8 +1609,9 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>52</v>
@@ -1549,8 +1625,9 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="5"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>53</v>
@@ -1564,8 +1641,9 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>54</v>
@@ -1579,8 +1657,9 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>55</v>
@@ -1594,8 +1673,9 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="5"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>56</v>
@@ -1609,8 +1689,9 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="5"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K57" s="5"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>57</v>
@@ -1624,8 +1705,9 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="5"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K58" s="5"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>58</v>
@@ -1639,8 +1721,9 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>59</v>
@@ -1654,8 +1737,9 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="5"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>60</v>
@@ -1669,8 +1753,9 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="5"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K61" s="5"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>61</v>
@@ -1684,8 +1769,9 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>62</v>
@@ -1699,8 +1785,9 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="5"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K63" s="5"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>63</v>
@@ -1714,8 +1801,9 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>64</v>
@@ -1729,8 +1817,9 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K65" s="5"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>65</v>
@@ -1744,8 +1833,9 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>66</v>
@@ -1759,8 +1849,9 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K67" s="5"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>67</v>
@@ -1774,8 +1865,9 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K68" s="5"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>68</v>
@@ -1789,8 +1881,9 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K69" s="5"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>69</v>
@@ -1804,8 +1897,9 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K70" s="5"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>70</v>
@@ -1819,8 +1913,9 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K71" s="5"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>71</v>
@@ -1834,8 +1929,9 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="5"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>72</v>
@@ -1849,8 +1945,9 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="5"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>73</v>
@@ -1864,8 +1961,9 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="5"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>74</v>
@@ -1879,8 +1977,9 @@
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="5"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>75</v>
@@ -1894,8 +1993,9 @@
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="5"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K76" s="5"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>76</v>
@@ -1909,8 +2009,9 @@
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="5"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K77" s="5"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>77</v>
@@ -1924,8 +2025,9 @@
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="5"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K78" s="5"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>78</v>
@@ -1939,8 +2041,9 @@
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="5"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K79" s="5"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>79</v>
@@ -1954,8 +2057,9 @@
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="5"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K80" s="5"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>80</v>
@@ -1969,8 +2073,9 @@
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="5"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K81" s="5"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>81</v>
@@ -1984,8 +2089,9 @@
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="J82" s="5"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K82" s="5"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>82</v>
@@ -1999,8 +2105,9 @@
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="5"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K83" s="5"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>83</v>
@@ -2014,8 +2121,9 @@
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="J84" s="5"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K84" s="5"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>84</v>
@@ -2029,8 +2137,9 @@
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="5"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K85" s="5"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>85</v>
@@ -2044,8 +2153,9 @@
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="5"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K86" s="5"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>86</v>
@@ -2059,8 +2169,9 @@
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="5"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>87</v>
@@ -2074,8 +2185,9 @@
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="5"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>88</v>
@@ -2089,8 +2201,9 @@
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="5"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K89" s="5"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>89</v>
@@ -2104,8 +2217,9 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="5"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A91">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>90</v>
@@ -2119,8 +2233,9 @@
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="5"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>91</v>
@@ -2134,8 +2249,9 @@
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="5"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A93">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>92</v>
@@ -2149,8 +2265,9 @@
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="J93" s="5"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K93" s="5"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>93</v>
@@ -2164,8 +2281,9 @@
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
       <c r="J94" s="5"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A95">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>94</v>
@@ -2179,8 +2297,9 @@
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="5"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K95" s="5"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>95</v>
@@ -2194,8 +2313,9 @@
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
       <c r="J96" s="5"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K96" s="5"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A97">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>96</v>
@@ -2209,8 +2329,9 @@
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="5"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K97" s="5"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A98">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>97</v>
@@ -2224,8 +2345,9 @@
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="5"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>98</v>
@@ -2239,8 +2361,9 @@
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="5"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K99" s="5"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>99</v>
@@ -2254,8 +2377,9 @@
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
       <c r="J100" s="5"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K100" s="5"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>100</v>
@@ -2269,8 +2393,9 @@
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="5"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K101" s="5"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>101</v>
@@ -2284,8 +2409,9 @@
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
       <c r="J102" s="5"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K102" s="5"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>102</v>
@@ -2299,8 +2425,9 @@
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
       <c r="J103" s="5"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K103" s="5"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>103</v>
@@ -2314,8 +2441,9 @@
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
       <c r="J104" s="5"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K104" s="5"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>104</v>
@@ -2329,8 +2457,9 @@
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
       <c r="J105" s="5"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K105" s="5"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A106">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>105</v>
@@ -2344,8 +2473,9 @@
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
       <c r="J106" s="5"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K106" s="5"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A107">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>106</v>
@@ -2359,8 +2489,9 @@
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="5"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K107" s="5"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A108">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>107</v>
@@ -2374,8 +2505,9 @@
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
       <c r="J108" s="5"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K108" s="5"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A109">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>108</v>
@@ -2389,8 +2521,9 @@
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
       <c r="J109" s="5"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K109" s="5"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>109</v>
@@ -2404,8 +2537,9 @@
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
       <c r="J110" s="5"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K110" s="5"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A111">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>110</v>
@@ -2419,8 +2553,9 @@
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="5"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K111" s="5"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A112">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>111</v>
@@ -2434,8 +2569,9 @@
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
       <c r="J112" s="5"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K112" s="5"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A113">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>112</v>
@@ -2449,8 +2585,9 @@
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
       <c r="J113" s="5"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K113" s="5"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A114">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>113</v>
@@ -2464,8 +2601,9 @@
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
       <c r="J114" s="5"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K114" s="5"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A115">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>114</v>
@@ -2479,8 +2617,9 @@
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
       <c r="J115" s="5"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K115" s="5"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A116">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>115</v>
@@ -2494,8 +2633,9 @@
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
       <c r="J116" s="5"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K116" s="5"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A117">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>116</v>
@@ -2509,8 +2649,9 @@
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
       <c r="J117" s="5"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K117" s="5"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A118">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>117</v>
@@ -2524,8 +2665,9 @@
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="5"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K118" s="5"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A119">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>118</v>
@@ -2539,8 +2681,9 @@
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
       <c r="J119" s="5"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K119" s="5"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A120">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>119</v>
@@ -2554,8 +2697,9 @@
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
       <c r="J120" s="5"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K120" s="5"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A121">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>120</v>
@@ -2569,8 +2713,9 @@
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
       <c r="J121" s="5"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K121" s="5"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A122">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>121</v>
@@ -2584,8 +2729,9 @@
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="5"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K122" s="5"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A123">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>122</v>
@@ -2599,8 +2745,9 @@
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="5"/>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K123" s="5"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A124">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>123</v>
@@ -2614,8 +2761,9 @@
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
       <c r="J124" s="5"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K124" s="5"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A125">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>124</v>
@@ -2629,8 +2777,9 @@
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="5"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K125" s="5"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A126">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>125</v>
@@ -2644,8 +2793,9 @@
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="5"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K126" s="5"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A127">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>126</v>
@@ -2659,8 +2809,9 @@
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="5"/>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K127" s="5"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A128">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>127</v>
@@ -2674,8 +2825,9 @@
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
       <c r="J128" s="5"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K128" s="5"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A129">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>128</v>
@@ -2689,8 +2841,9 @@
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
       <c r="J129" s="5"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K129" s="5"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A130">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>129</v>
@@ -2704,8 +2857,9 @@
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
       <c r="J130" s="5"/>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K130" s="5"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A131">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>130</v>
@@ -2719,8 +2873,9 @@
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
       <c r="J131" s="5"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K131" s="5"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A132">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>131</v>
@@ -2734,8 +2889,9 @@
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
       <c r="J132" s="5"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K132" s="5"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A133">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>132</v>
@@ -2749,8 +2905,9 @@
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="5"/>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K133" s="5"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A134">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>133</v>
@@ -2764,8 +2921,9 @@
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
       <c r="J134" s="5"/>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K134" s="5"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A135">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>134</v>
@@ -2779,8 +2937,9 @@
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
       <c r="J135" s="5"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K135" s="5"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A136">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>135</v>
@@ -2794,8 +2953,9 @@
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
       <c r="J136" s="5"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K136" s="5"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A137">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>136</v>
@@ -2809,8 +2969,9 @@
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
       <c r="J137" s="5"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K137" s="5"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A138">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>137</v>
@@ -2824,8 +2985,9 @@
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
       <c r="J138" s="5"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K138" s="5"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A139">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>138</v>
@@ -2839,8 +3001,9 @@
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
       <c r="J139" s="5"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K139" s="5"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A140">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>139</v>
@@ -2854,8 +3017,9 @@
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
       <c r="J140" s="5"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K140" s="5"/>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A141">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>140</v>
@@ -2869,8 +3033,9 @@
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
       <c r="J141" s="5"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K141" s="5"/>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A142">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>141</v>
@@ -2884,8 +3049,9 @@
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
       <c r="J142" s="5"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K142" s="5"/>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A143">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>142</v>
@@ -2899,8 +3065,9 @@
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
       <c r="J143" s="5"/>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K143" s="5"/>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A144">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>143</v>
@@ -2914,8 +3081,9 @@
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
       <c r="J144" s="5"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K144" s="5"/>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A145">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>144</v>
@@ -2929,8 +3097,9 @@
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
       <c r="J145" s="5"/>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K145" s="5"/>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A146">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>145</v>
@@ -2944,8 +3113,9 @@
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
       <c r="J146" s="5"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K146" s="5"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A147">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>146</v>
@@ -2959,8 +3129,9 @@
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
       <c r="J147" s="5"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K147" s="5"/>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A148">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>147</v>
@@ -2974,8 +3145,9 @@
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
       <c r="J148" s="5"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K148" s="5"/>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A149">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>148</v>
@@ -2989,8 +3161,9 @@
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
       <c r="J149" s="5"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K149" s="5"/>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A150">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>149</v>
@@ -3004,8 +3177,9 @@
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
       <c r="J150" s="5"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K150" s="5"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A151">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>150</v>
@@ -3019,8 +3193,9 @@
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
       <c r="J151" s="5"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K151" s="5"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A152">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>151</v>
@@ -3034,8 +3209,9 @@
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
       <c r="J152" s="5"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K152" s="5"/>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A153">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>152</v>
@@ -3049,8 +3225,9 @@
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
       <c r="J153" s="5"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K153" s="5"/>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A154">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>153</v>
@@ -3064,8 +3241,9 @@
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
       <c r="J154" s="5"/>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K154" s="5"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A155">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>154</v>
@@ -3079,8 +3257,9 @@
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
       <c r="J155" s="5"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K155" s="5"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A156">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>155</v>
@@ -3094,8 +3273,9 @@
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
       <c r="J156" s="5"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K156" s="5"/>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A157">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>156</v>
@@ -3109,8 +3289,9 @@
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
       <c r="J157" s="5"/>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K157" s="5"/>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A158">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>157</v>
@@ -3124,8 +3305,9 @@
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
       <c r="J158" s="5"/>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K158" s="5"/>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A159">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>158</v>
@@ -3139,8 +3321,9 @@
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
       <c r="J159" s="5"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K159" s="5"/>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A160">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>159</v>
@@ -3154,8 +3337,9 @@
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
       <c r="J160" s="5"/>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K160" s="5"/>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A161">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>160</v>
@@ -3169,8 +3353,9 @@
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
       <c r="J161" s="5"/>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K161" s="5"/>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A162">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>161</v>
@@ -3184,8 +3369,9 @@
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
       <c r="J162" s="5"/>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K162" s="5"/>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A163">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>162</v>
@@ -3199,8 +3385,9 @@
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
       <c r="J163" s="5"/>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K163" s="5"/>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A164">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>163</v>
@@ -3214,8 +3401,9 @@
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
       <c r="J164" s="5"/>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K164" s="5"/>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A165">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>164</v>
@@ -3229,8 +3417,9 @@
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
       <c r="J165" s="5"/>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K165" s="5"/>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A166">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>165</v>
@@ -3244,8 +3433,9 @@
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
       <c r="J166" s="5"/>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K166" s="5"/>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A167">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>166</v>
@@ -3259,8 +3449,9 @@
       <c r="H167" s="3"/>
       <c r="I167" s="3"/>
       <c r="J167" s="5"/>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K167" s="5"/>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A168">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>167</v>
@@ -3274,8 +3465,9 @@
       <c r="H168" s="3"/>
       <c r="I168" s="3"/>
       <c r="J168" s="5"/>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K168" s="5"/>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A169">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>168</v>
@@ -3289,8 +3481,9 @@
       <c r="H169" s="3"/>
       <c r="I169" s="3"/>
       <c r="J169" s="5"/>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K169" s="5"/>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A170">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>169</v>
@@ -3304,8 +3497,9 @@
       <c r="H170" s="3"/>
       <c r="I170" s="3"/>
       <c r="J170" s="5"/>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K170" s="5"/>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A171">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>170</v>
@@ -3319,8 +3513,9 @@
       <c r="H171" s="3"/>
       <c r="I171" s="3"/>
       <c r="J171" s="5"/>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K171" s="5"/>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A172">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>171</v>
@@ -3334,8 +3529,9 @@
       <c r="H172" s="3"/>
       <c r="I172" s="3"/>
       <c r="J172" s="5"/>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K172" s="5"/>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A173">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>172</v>
@@ -3349,8 +3545,9 @@
       <c r="H173" s="3"/>
       <c r="I173" s="3"/>
       <c r="J173" s="5"/>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K173" s="5"/>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A174">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>173</v>
@@ -3364,8 +3561,9 @@
       <c r="H174" s="3"/>
       <c r="I174" s="3"/>
       <c r="J174" s="5"/>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K174" s="5"/>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A175">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>174</v>
@@ -3379,8 +3577,9 @@
       <c r="H175" s="3"/>
       <c r="I175" s="3"/>
       <c r="J175" s="5"/>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K175" s="5"/>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A176">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>175</v>
@@ -3394,8 +3593,9 @@
       <c r="H176" s="3"/>
       <c r="I176" s="3"/>
       <c r="J176" s="5"/>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K176" s="5"/>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A177">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>176</v>
@@ -3409,8 +3609,9 @@
       <c r="H177" s="3"/>
       <c r="I177" s="3"/>
       <c r="J177" s="5"/>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K177" s="5"/>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A178">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>177</v>
@@ -3424,8 +3625,9 @@
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
       <c r="J178" s="5"/>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K178" s="5"/>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A179">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>178</v>
@@ -3439,8 +3641,9 @@
       <c r="H179" s="3"/>
       <c r="I179" s="3"/>
       <c r="J179" s="5"/>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K179" s="5"/>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A180">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>179</v>
@@ -3454,8 +3657,9 @@
       <c r="H180" s="3"/>
       <c r="I180" s="3"/>
       <c r="J180" s="5"/>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K180" s="5"/>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A181">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>180</v>
@@ -3469,8 +3673,9 @@
       <c r="H181" s="3"/>
       <c r="I181" s="3"/>
       <c r="J181" s="5"/>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K181" s="5"/>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A182">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>181</v>
@@ -3484,8 +3689,9 @@
       <c r="H182" s="3"/>
       <c r="I182" s="3"/>
       <c r="J182" s="5"/>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K182" s="5"/>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A183">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>182</v>
@@ -3499,8 +3705,9 @@
       <c r="H183" s="3"/>
       <c r="I183" s="3"/>
       <c r="J183" s="5"/>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K183" s="5"/>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A184">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>183</v>
@@ -3514,8 +3721,9 @@
       <c r="H184" s="3"/>
       <c r="I184" s="3"/>
       <c r="J184" s="5"/>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K184" s="5"/>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A185">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>184</v>
@@ -3529,8 +3737,9 @@
       <c r="H185" s="3"/>
       <c r="I185" s="3"/>
       <c r="J185" s="5"/>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K185" s="5"/>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A186">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>185</v>
@@ -3544,8 +3753,9 @@
       <c r="H186" s="3"/>
       <c r="I186" s="3"/>
       <c r="J186" s="5"/>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K186" s="5"/>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A187">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>186</v>
@@ -3559,8 +3769,9 @@
       <c r="H187" s="3"/>
       <c r="I187" s="3"/>
       <c r="J187" s="5"/>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K187" s="5"/>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A188">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>187</v>
@@ -3574,8 +3785,9 @@
       <c r="H188" s="3"/>
       <c r="I188" s="3"/>
       <c r="J188" s="5"/>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K188" s="5"/>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A189">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>188</v>
@@ -3589,8 +3801,9 @@
       <c r="H189" s="3"/>
       <c r="I189" s="3"/>
       <c r="J189" s="5"/>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K189" s="5"/>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A190">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>189</v>
@@ -3604,8 +3817,9 @@
       <c r="H190" s="3"/>
       <c r="I190" s="3"/>
       <c r="J190" s="5"/>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K190" s="5"/>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A191">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>190</v>
@@ -3619,8 +3833,9 @@
       <c r="H191" s="3"/>
       <c r="I191" s="3"/>
       <c r="J191" s="5"/>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K191" s="5"/>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A192">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>191</v>
@@ -3634,8 +3849,9 @@
       <c r="H192" s="3"/>
       <c r="I192" s="3"/>
       <c r="J192" s="5"/>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K192" s="5"/>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A193">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>192</v>
@@ -3649,8 +3865,9 @@
       <c r="H193" s="3"/>
       <c r="I193" s="3"/>
       <c r="J193" s="5"/>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K193" s="5"/>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A194">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>193</v>
@@ -3664,8 +3881,9 @@
       <c r="H194" s="3"/>
       <c r="I194" s="3"/>
       <c r="J194" s="5"/>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K194" s="5"/>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A195">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>194</v>
@@ -3679,8 +3897,9 @@
       <c r="H195" s="3"/>
       <c r="I195" s="3"/>
       <c r="J195" s="5"/>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K195" s="5"/>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A196">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>195</v>
@@ -3694,8 +3913,9 @@
       <c r="H196" s="3"/>
       <c r="I196" s="3"/>
       <c r="J196" s="5"/>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K196" s="5"/>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A197">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>196</v>
@@ -3709,8 +3929,9 @@
       <c r="H197" s="3"/>
       <c r="I197" s="3"/>
       <c r="J197" s="5"/>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K197" s="5"/>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A198">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>197</v>
@@ -3724,8 +3945,9 @@
       <c r="H198" s="3"/>
       <c r="I198" s="3"/>
       <c r="J198" s="5"/>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K198" s="5"/>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A199">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>198</v>
@@ -3739,8 +3961,9 @@
       <c r="H199" s="3"/>
       <c r="I199" s="3"/>
       <c r="J199" s="5"/>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K199" s="5"/>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A200">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>199</v>
@@ -3754,8 +3977,9 @@
       <c r="H200" s="3"/>
       <c r="I200" s="3"/>
       <c r="J200" s="5"/>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K200" s="5"/>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A201">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>200</v>
@@ -3769,8 +3993,9 @@
       <c r="H201" s="3"/>
       <c r="I201" s="3"/>
       <c r="J201" s="5"/>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K201" s="5"/>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A202">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>201</v>
@@ -3784,8 +4009,9 @@
       <c r="H202" s="3"/>
       <c r="I202" s="3"/>
       <c r="J202" s="5"/>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K202" s="5"/>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A203">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>202</v>
@@ -3799,8 +4025,9 @@
       <c r="H203" s="3"/>
       <c r="I203" s="3"/>
       <c r="J203" s="5"/>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K203" s="5"/>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A204">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>203</v>
@@ -3814,8 +4041,9 @@
       <c r="H204" s="3"/>
       <c r="I204" s="3"/>
       <c r="J204" s="5"/>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K204" s="5"/>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A205">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>204</v>
@@ -3829,8 +4057,9 @@
       <c r="H205" s="3"/>
       <c r="I205" s="3"/>
       <c r="J205" s="5"/>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K205" s="5"/>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A206">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>205</v>
@@ -3844,8 +4073,9 @@
       <c r="H206" s="3"/>
       <c r="I206" s="3"/>
       <c r="J206" s="5"/>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K206" s="5"/>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A207">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>206</v>
@@ -3859,8 +4089,9 @@
       <c r="H207" s="3"/>
       <c r="I207" s="3"/>
       <c r="J207" s="5"/>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K207" s="5"/>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A208">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>207</v>
@@ -3874,8 +4105,9 @@
       <c r="H208" s="3"/>
       <c r="I208" s="3"/>
       <c r="J208" s="5"/>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K208" s="5"/>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A209">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>208</v>
@@ -3889,8 +4121,9 @@
       <c r="H209" s="3"/>
       <c r="I209" s="3"/>
       <c r="J209" s="5"/>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K209" s="5"/>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A210">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>209</v>
@@ -3904,8 +4137,9 @@
       <c r="H210" s="3"/>
       <c r="I210" s="3"/>
       <c r="J210" s="5"/>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K210" s="5"/>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A211">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>210</v>
@@ -3919,8 +4153,9 @@
       <c r="H211" s="3"/>
       <c r="I211" s="3"/>
       <c r="J211" s="5"/>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K211" s="5"/>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A212">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>211</v>
@@ -3934,8 +4169,9 @@
       <c r="H212" s="3"/>
       <c r="I212" s="3"/>
       <c r="J212" s="5"/>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K212" s="5"/>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A213">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>212</v>
@@ -3949,8 +4185,9 @@
       <c r="H213" s="3"/>
       <c r="I213" s="3"/>
       <c r="J213" s="5"/>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K213" s="5"/>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A214">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>213</v>
@@ -3964,8 +4201,9 @@
       <c r="H214" s="3"/>
       <c r="I214" s="3"/>
       <c r="J214" s="5"/>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K214" s="5"/>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A215">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>214</v>
@@ -3979,8 +4217,9 @@
       <c r="H215" s="3"/>
       <c r="I215" s="3"/>
       <c r="J215" s="5"/>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K215" s="5"/>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A216">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>215</v>
@@ -3994,8 +4233,9 @@
       <c r="H216" s="3"/>
       <c r="I216" s="3"/>
       <c r="J216" s="5"/>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K216" s="5"/>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A217">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>216</v>
@@ -4009,8 +4249,9 @@
       <c r="H217" s="3"/>
       <c r="I217" s="3"/>
       <c r="J217" s="5"/>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K217" s="5"/>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A218">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>217</v>
@@ -4024,8 +4265,9 @@
       <c r="H218" s="3"/>
       <c r="I218" s="3"/>
       <c r="J218" s="5"/>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K218" s="5"/>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A219">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>218</v>
@@ -4039,8 +4281,9 @@
       <c r="H219" s="3"/>
       <c r="I219" s="3"/>
       <c r="J219" s="5"/>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K219" s="5"/>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A220">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>219</v>
@@ -4054,8 +4297,9 @@
       <c r="H220" s="3"/>
       <c r="I220" s="3"/>
       <c r="J220" s="5"/>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K220" s="5"/>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A221">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>220</v>
@@ -4069,8 +4313,9 @@
       <c r="H221" s="3"/>
       <c r="I221" s="3"/>
       <c r="J221" s="5"/>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K221" s="5"/>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A222">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>221</v>
@@ -4084,8 +4329,9 @@
       <c r="H222" s="3"/>
       <c r="I222" s="3"/>
       <c r="J222" s="5"/>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K222" s="5"/>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A223">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>222</v>
@@ -4099,8 +4345,9 @@
       <c r="H223" s="3"/>
       <c r="I223" s="3"/>
       <c r="J223" s="5"/>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K223" s="5"/>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A224">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>223</v>
@@ -4114,8 +4361,9 @@
       <c r="H224" s="3"/>
       <c r="I224" s="3"/>
       <c r="J224" s="5"/>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K224" s="5"/>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A225">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>224</v>
@@ -4129,8 +4377,9 @@
       <c r="H225" s="3"/>
       <c r="I225" s="3"/>
       <c r="J225" s="5"/>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K225" s="5"/>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A226">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>225</v>
@@ -4144,8 +4393,9 @@
       <c r="H226" s="3"/>
       <c r="I226" s="3"/>
       <c r="J226" s="5"/>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K226" s="5"/>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A227">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>226</v>
@@ -4159,8 +4409,9 @@
       <c r="H227" s="3"/>
       <c r="I227" s="3"/>
       <c r="J227" s="5"/>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K227" s="5"/>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A228">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>227</v>
@@ -4174,8 +4425,9 @@
       <c r="H228" s="3"/>
       <c r="I228" s="3"/>
       <c r="J228" s="5"/>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K228" s="5"/>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A229">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>228</v>
@@ -4189,8 +4441,9 @@
       <c r="H229" s="3"/>
       <c r="I229" s="3"/>
       <c r="J229" s="5"/>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K229" s="5"/>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A230">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>229</v>
@@ -4204,8 +4457,9 @@
       <c r="H230" s="3"/>
       <c r="I230" s="3"/>
       <c r="J230" s="5"/>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K230" s="5"/>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A231">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>230</v>
@@ -4219,8 +4473,9 @@
       <c r="H231" s="3"/>
       <c r="I231" s="3"/>
       <c r="J231" s="5"/>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K231" s="5"/>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A232">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>231</v>
@@ -4234,8 +4489,9 @@
       <c r="H232" s="3"/>
       <c r="I232" s="3"/>
       <c r="J232" s="5"/>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K232" s="5"/>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A233">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>232</v>
@@ -4249,8 +4505,9 @@
       <c r="H233" s="3"/>
       <c r="I233" s="3"/>
       <c r="J233" s="5"/>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K233" s="5"/>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A234">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>233</v>
@@ -4264,8 +4521,9 @@
       <c r="H234" s="3"/>
       <c r="I234" s="3"/>
       <c r="J234" s="5"/>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K234" s="5"/>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A235">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>234</v>
@@ -4279,8 +4537,9 @@
       <c r="H235" s="3"/>
       <c r="I235" s="3"/>
       <c r="J235" s="5"/>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K235" s="5"/>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A236">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>235</v>
@@ -4294,8 +4553,9 @@
       <c r="H236" s="3"/>
       <c r="I236" s="3"/>
       <c r="J236" s="5"/>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K236" s="5"/>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A237">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>236</v>
@@ -4309,8 +4569,9 @@
       <c r="H237" s="3"/>
       <c r="I237" s="3"/>
       <c r="J237" s="5"/>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K237" s="5"/>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A238">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>237</v>
@@ -4324,8 +4585,9 @@
       <c r="H238" s="3"/>
       <c r="I238" s="3"/>
       <c r="J238" s="5"/>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K238" s="5"/>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A239">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>238</v>
@@ -4339,8 +4601,9 @@
       <c r="H239" s="3"/>
       <c r="I239" s="3"/>
       <c r="J239" s="5"/>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K239" s="5"/>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A240">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>239</v>
@@ -4354,8 +4617,9 @@
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
       <c r="J240" s="5"/>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K240" s="5"/>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A241">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>240</v>
@@ -4369,8 +4633,9 @@
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="5"/>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K241" s="5"/>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A242">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>241</v>
@@ -4384,8 +4649,9 @@
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
       <c r="J242" s="5"/>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K242" s="5"/>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A243">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>242</v>
@@ -4399,8 +4665,9 @@
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
       <c r="J243" s="5"/>
-    </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K243" s="5"/>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A244">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>243</v>
@@ -4414,8 +4681,9 @@
       <c r="H244" s="3"/>
       <c r="I244" s="3"/>
       <c r="J244" s="5"/>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K244" s="5"/>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A245">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>244</v>
@@ -4429,8 +4697,9 @@
       <c r="H245" s="3"/>
       <c r="I245" s="3"/>
       <c r="J245" s="5"/>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K245" s="5"/>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A246">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>245</v>
@@ -4444,8 +4713,9 @@
       <c r="H246" s="3"/>
       <c r="I246" s="3"/>
       <c r="J246" s="5"/>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K246" s="5"/>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A247">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>246</v>
@@ -4459,8 +4729,9 @@
       <c r="H247" s="3"/>
       <c r="I247" s="3"/>
       <c r="J247" s="5"/>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K247" s="5"/>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A248">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>247</v>
@@ -4474,8 +4745,9 @@
       <c r="H248" s="3"/>
       <c r="I248" s="3"/>
       <c r="J248" s="5"/>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K248" s="5"/>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A249">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>248</v>
@@ -4489,8 +4761,9 @@
       <c r="H249" s="3"/>
       <c r="I249" s="3"/>
       <c r="J249" s="5"/>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K249" s="5"/>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A250">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>249</v>
@@ -4504,8 +4777,9 @@
       <c r="H250" s="3"/>
       <c r="I250" s="3"/>
       <c r="J250" s="5"/>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="K250" s="5"/>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A251">
         <f>ROW()-ROW(Table3[[#Headers],[S/N]])</f>
         <v>250</v>
@@ -4519,8 +4793,9 @@
       <c r="H251" s="4"/>
       <c r="I251" s="4"/>
       <c r="J251" s="5"/>
-    </row>
-    <row r="253" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.65"/>
+      <c r="K251" s="5"/>
+    </row>
+    <row r="253" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>